<commit_message>
for ghb initial only problem management
</commit_message>
<xml_diff>
--- a/wwwroot/TermProbExcel/InputTemplate/CheckProblemDevice.xlsx
+++ b/wwwroot/TermProbExcel/InputTemplate/CheckProblemDevice.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26903"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\SLA_Management\wwwroot\TermProbExcel\excelfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C42D4E0-8522-4F89-A48E-AF28FF621CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="19875" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceTermProb" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DeviceTermProb!$A$7:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -44,28 +58,28 @@
     <t>Seq No.</t>
   </si>
   <si>
-    <t>Branch Name</t>
+    <t>Date Time</t>
+  </si>
+  <si>
+    <t>Serial No</t>
   </si>
   <si>
     <t>Terminal ID</t>
   </si>
   <si>
+    <t>Terminal Name</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Problem Name</t>
-  </si>
-  <si>
-    <t>Remark</t>
-  </si>
-  <si>
-    <t>Date Time</t>
+    <t>Event Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -143,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,15 +169,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,9 +200,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,9 +240,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,7 +312,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,28 +485,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="65" style="1" customWidth="1"/>
+    <col min="7" max="7" width="43.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="18">
-      <c r="A2" s="7"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -501,14 +514,14 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" ht="18">
-      <c r="A3" s="7"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+    <row r="3" spans="1:12" ht="18">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -516,10 +529,10 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -527,7 +540,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -568,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -580,7 +593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Update excel in deviceTermProb
</commit_message>
<xml_diff>
--- a/wwwroot/TermProbExcel/InputTemplate/CheckProblemDevice.xlsx
+++ b/wwwroot/TermProbExcel/InputTemplate/CheckProblemDevice.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>จากวันที่</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Event Name</t>
+  </si>
+  <si>
+    <t>Event Desciption</t>
   </si>
 </sst>
 </file>
@@ -142,11 +145,11 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="1" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -379,7 +382,8 @@
     <col customWidth="1" min="5" max="5" width="39.25"/>
     <col customWidth="1" min="6" max="6" width="65.0"/>
     <col customWidth="1" min="7" max="7" width="43.63"/>
-    <col customWidth="1" min="8" max="12" width="9.0"/>
+    <col customWidth="1" min="8" max="8" width="45.0"/>
+    <col customWidth="1" min="9" max="12" width="9.0"/>
     <col customWidth="1" min="13" max="26" width="8.63"/>
   </cols>
   <sheetData>
@@ -490,7 +494,7 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
@@ -550,28 +554,30 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>

</xml_diff>